<commit_message>
fix: empty rows in xlsx
</commit_message>
<xml_diff>
--- a/testcases/employees_all.xlsx
+++ b/testcases/employees_all.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="employees"/>
@@ -129,7 +129,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -172,9 +172,6 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -193,8 +190,11 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,10 +504,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -531,7 +531,7 @@
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>2000</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -545,7 +545,7 @@
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>1000</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -559,7 +559,7 @@
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>1309432</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -573,7 +573,7 @@
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>5000</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -587,7 +587,7 @@
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>4000</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -601,7 +601,7 @@
       <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>3000</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -615,7 +615,7 @@
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>2499</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -629,7 +629,7 @@
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>900</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -643,7 +643,7 @@
       <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>4000</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -666,10 +666,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -693,7 +693,7 @@
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>2000</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -707,7 +707,7 @@
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>2499</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -726,153 +726,153 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>2499</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>2499</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>2501</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>2501</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>2500</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>2501</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>1</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>2499</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>2500</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -886,71 +886,59 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>2499</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
+      <c r="D3" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -968,10 +956,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -995,7 +983,7 @@
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>2499</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1009,7 +997,7 @@
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>2499</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1032,10 +1020,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1059,7 +1047,7 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>2499</v>
       </c>
       <c r="D2" s="1" t="s">

</xml_diff>